<commit_message>
Channels with integration problems running in NEURON
</commit_message>
<xml_diff>
--- a/Import Scripts/voltageClamp/channelModelManager.xlsx
+++ b/Import Scripts/voltageClamp/channelModelManager.xlsx
@@ -14,7 +14,7 @@
     <sheet name="problemChannels" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">problemChannels!$A$1:$C$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">problemChannels!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$141</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$F$141</definedName>
   </definedNames>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="735">
   <si>
     <t>/www/NeuroMLmodels/NMLCH000001/hd.nml</t>
   </si>
@@ -2163,61 +2163,76 @@
     <t>NMLCH000035/CaT_Chan.nml</t>
   </si>
   <si>
-    <t>NMLCH000036/CaPool.nml</t>
-  </si>
-  <si>
     <t>NMLCH000037/CaP_Chan.nml</t>
   </si>
   <si>
-    <t>NMLCH000051/cad.nml</t>
-  </si>
-  <si>
-    <t>NMLCH000133/IT.channel.nml</t>
-  </si>
-  <si>
-    <t>NMLCH000152/kc_fast.channel.nml</t>
-  </si>
-  <si>
-    <t>NMLCH000153/kc.channel.nml</t>
-  </si>
-  <si>
     <t>Channel</t>
   </si>
   <si>
     <t>Problem</t>
   </si>
   <si>
-    <t>DeShutter&amp;Bower channels that were in NMLv1.8 format. PG's NMLv1.8-&gt;NML2 converter does not support the format used in the NMLv1.8 files. Conversion results in .nml files that say "Not implemented yet"</t>
-  </si>
-  <si>
     <t>Can't convert from NMLv1.8 to v2</t>
   </si>
   <si>
-    <t>Does not validate, but seems to run OK</t>
-  </si>
-  <si>
-    <t>Traub TMC model. Tag "baseConductanceScalingCaDependent" used in channel does not appear to be part of NML2</t>
-  </si>
-  <si>
-    <t>Covered by existing issue from 1yr ago: https://github.com/OpenSourceBrain/Thalamocortical/issues/7</t>
-  </si>
-  <si>
-    <t>Does not validate, shows I&amp;G =0</t>
-  </si>
-  <si>
-    <t>Ca pool model</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
     <t>Example of NMLv1.8 version file that the converter does not support: https://github.com/scrook/neuroml-db/blob/e4f088fdcd3ddeb7b99fbeeff70cc5e40681e3b1/www/NeuroMLmodels/NMLCH000025/NaP_Chan.xml</t>
   </si>
   <si>
-    <t>Created an issue: https://github.com/OpenSourceBrain/PurkinjeCell/issues/2</t>
-  </si>
-  <si>
-    <t>Pospischil model. Validator complains about 'IT_s_gate' type that is defined later in the channel. Have to investigate why it works OK as part of a cell, but not in our test protocol.</t>
+    <t>NMLCH000009</t>
+  </si>
+  <si>
+    <t>NMLCH000022</t>
+  </si>
+  <si>
+    <t>NMLCH000097</t>
+  </si>
+  <si>
+    <t>NMLCH000098</t>
+  </si>
+  <si>
+    <t>NMLCH000105</t>
+  </si>
+  <si>
+    <t>NMLCH000116</t>
+  </si>
+  <si>
+    <t>NMLCH000117</t>
+  </si>
+  <si>
+    <t>NMLCH000126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infinite values integration problems </t>
+  </si>
+  <si>
+    <t>DeSchutter&amp;Bower channels that were in NMLv1.8 format. PG's NMLv1.8-&gt;NML2 converter does not support the format used in the NMLv1.8 files. Conversion results in .nml files that say "Not implemented yet"</t>
+  </si>
+  <si>
+    <t>Inactivation integration probs</t>
+  </si>
+  <si>
+    <t>Numerical instabilities</t>
+  </si>
+  <si>
+    <t>Inactivation and deactivation probs</t>
+  </si>
+  <si>
+    <t>Converted to NEURON</t>
+  </si>
+  <si>
+    <t>Leaving these as is -- other channels work fine with the protocol</t>
+  </si>
+  <si>
+    <t>Indicates that problem is with channels</t>
+  </si>
+  <si>
+    <t>Created an issue. No response as of 6/2/17 https://github.com/OpenSourceBrain/PurkinjeCell/issues/2</t>
+  </si>
+  <si>
+    <t>Still various problems with channels, despite NEURON &amp; small dt</t>
   </si>
 </sst>
 </file>
@@ -2265,7 +2280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2322,32 +2337,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2379,19 +2368,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="435">
+  <cellStyleXfs count="443">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2827,8 +2805,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2844,40 +2830,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2886,34 +2883,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="435">
+  <cellStyles count="443">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3131,6 +3108,10 @@
     <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3348,6 +3329,10 @@
     <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3679,7 +3664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView topLeftCell="I42" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
@@ -13827,10 +13812,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="A12" sqref="A12:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13873,6 +13858,46 @@
     <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>724</v>
       </c>
     </row>
   </sheetData>
@@ -13888,10 +13913,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13902,13 +13927,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="B1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="C1" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -13916,227 +13941,240 @@
         <v>701</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>720</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>719</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
+        <v>714</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="21"/>
+      <c r="B3" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="21"/>
+      <c r="B4" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>704</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="21"/>
+      <c r="B5" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>705</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="21"/>
+      <c r="B6" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>706</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>727</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="21"/>
+      <c r="B7" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>716</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
+      <c r="B8" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>708</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="21"/>
+      <c r="B9" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>709</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="21"/>
+      <c r="B10" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>710</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="14"/>
+      <c r="B11" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>733</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>711</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>725</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>728</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="9" t="s">
-        <v>712</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>720</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
+      <c r="C13" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="11" t="s">
-        <v>713</v>
-      </c>
-      <c r="B14" s="12" t="s">
+        <v>718</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>728</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>734</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="11" t="s">
+        <v>720</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>729</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1">
+      <c r="A16" s="11" t="s">
+        <v>721</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>728</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="11" t="s">
+        <v>722</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>727</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="47" customHeight="1">
-      <c r="A15" s="11" t="s">
-        <v>714</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>724</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>729</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
-    </row>
-    <row r="16" spans="1:7" ht="37" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>715</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>721</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>722</v>
-      </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="35"/>
-    </row>
-    <row r="17" spans="1:7" ht="41" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>716</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>721</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>723</v>
-      </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
     </row>
   </sheetData>
   <sortState ref="A20:B45">
     <sortCondition ref="A20"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="C2:G6"/>
     <mergeCell ref="C7:G10"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C12:G13"/>
+    <mergeCell ref="C11:G12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>